<commit_message>
XML root node is specified in metatab instead
</commit_message>
<xml_diff>
--- a/flattentool/tests/fixtures/xlsx/iati-org.xlsx
+++ b/flattentool/tests/fixtures/xlsx/iati-org.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19316"/>
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="main" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="main" sheetId="1" r:id="rId1"/>
+    <sheet name="Meta" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="179016"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>organisation-identifier</t>
   </si>
@@ -36,25 +36,30 @@
   </si>
   <si>
     <t>40</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>XMLRootPath iati-organisations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -70,15 +75,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -366,18 +380,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -408,6 +416,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A433AB37-B13C-475C-8688-69A5D8E50C37}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{8642BCCC-7C95-5A81-8932-E30EDBEB35BF}">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update XLSX fixture to use XMLRootTag
</commit_message>
<xml_diff>
--- a/flattentool/tests/fixtures/xlsx/iati-org.xlsx
+++ b/flattentool/tests/fixtures/xlsx/iati-org.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19316"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19310"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <t>#</t>
   </si>
   <si>
-    <t>XMLRootPath iati-organisations</t>
+    <t>XMLRootTag iati-organisations</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Add a test for specifying RootListPath via metatab
</commit_message>
<xml_diff>
--- a/flattentool/tests/fixtures/xlsx/iati-org.xlsx
+++ b/flattentool/tests/fixtures/xlsx/iati-org.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>organisation-identifier</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>XMLRootTag iati-organisations</t>
+  </si>
+  <si>
+    <t>RootListPath iati-organisation</t>
   </si>
 </sst>
 </file>
@@ -422,20 +425,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A433AB37-B13C-475C-8688-69A5D8E50C37}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{8642BCCC-7C95-5A81-8932-E30EDBEB35BF}">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>